<commit_message>
Fill nan with empty string after merging data frames and add default row name for testing.
</commit_message>
<xml_diff>
--- a/app/_resources/default_krbiz_delivery_format.xlsx
+++ b/app/_resources/default_krbiz_delivery_format.xlsx
@@ -493,7 +493,7 @@
     <col min="2" max="2" style="8" width="19.719285714285714" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="8" width="28.005" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="9" width="24.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="36.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="15.147857142857141" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="8" width="18.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="8" width="13.005" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="8" width="22.576428571428572" customWidth="1" bestFit="1"/>
@@ -529,7 +529,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>